<commit_message>
Lamination is selected, motor dimensions are determined.
</commit_message>
<xml_diff>
--- a/Project 2/Winding Design.xlsx
+++ b/Project 2/Winding Design.xlsx
@@ -4,14 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Winding Design" sheetId="1" r:id="rId1"/>
+    <sheet name="Motor Parameter Estimation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -22,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="110">
   <si>
     <t>A</t>
   </si>
@@ -315,10 +313,43 @@
     <t>Integral, Double Layer, Distributed Winding</t>
   </si>
   <si>
-    <t>14AWG</t>
-  </si>
-  <si>
     <t>coil span=120 (6 slots)</t>
+  </si>
+  <si>
+    <t>Axial Length (mm)</t>
+  </si>
+  <si>
+    <t>16AWG</t>
+  </si>
+  <si>
+    <t>A (mm)</t>
+  </si>
+  <si>
+    <t>Bavg(T)</t>
+  </si>
+  <si>
+    <t>Specific Electric Loading-q (A/m)</t>
+  </si>
+  <si>
+    <t>Full-Load Efficiency</t>
+  </si>
+  <si>
+    <t>Full-Load Power Factor</t>
+  </si>
+  <si>
+    <t>Output Coefficient</t>
+  </si>
+  <si>
+    <t>ns (rps)</t>
+  </si>
+  <si>
+    <t>D^2.L(m^3)</t>
+  </si>
+  <si>
+    <t>L (m)</t>
+  </si>
+  <si>
+    <t>Di (m)</t>
   </si>
 </sst>
 </file>
@@ -432,11 +463,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -450,6 +478,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,7 +494,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,7 +631,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$21:$D$40</c:f>
+              <c:f>'Winding Design'!$D$21:$D$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -663,7 +700,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$21:$E$40</c:f>
+              <c:f>'Winding Design'!$E$21:$E$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -769,7 +806,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$21:$D$40</c:f>
+              <c:f>'Winding Design'!$D$21:$D$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -838,7 +875,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$21:$F$40</c:f>
+              <c:f>'Winding Design'!$F$21:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1959,102 +1996,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="H3">
-            <v>97.700486994000997</v>
-          </cell>
-          <cell r="I3">
-            <v>0.01</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="H4">
-            <v>98.815801553305064</v>
-          </cell>
-          <cell r="I4">
-            <v>0.02</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="H5">
-            <v>98.868518908576021</v>
-          </cell>
-          <cell r="I5">
-            <v>0.03</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="H6">
-            <v>98.748992430368304</v>
-          </cell>
-          <cell r="I6">
-            <v>0.04</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="H7">
-            <v>98.575513293573863</v>
-          </cell>
-          <cell r="I7">
-            <v>0.05</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="H33">
-            <v>97.303714017042296</v>
-          </cell>
-          <cell r="I33">
-            <v>0.01</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="H34">
-            <v>98.675830030787097</v>
-          </cell>
-          <cell r="I34">
-            <v>0.02</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="H35">
-            <v>98.79763956212048</v>
-          </cell>
-          <cell r="I35">
-            <v>0.03</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="H36">
-            <v>98.709563864053138</v>
-          </cell>
-          <cell r="I36">
-            <v>0.04</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="H37">
-            <v>98.553964696817815</v>
-          </cell>
-          <cell r="I37">
-            <v>0.05</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2320,1122 +2261,1144 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="6"/>
-    <col min="7" max="7" width="9.140625" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="6" width="9.140625" style="5"/>
+    <col min="7" max="7" width="9.140625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="7">
+      <c r="B1" s="14"/>
+      <c r="C1" s="6">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="7">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="6">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="J2" s="8" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="J2" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="7">
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="6">
         <f>M1/C1</f>
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="7">
+      <c r="B3" s="14"/>
+      <c r="C3" s="6">
         <f>SIN(M3*N4/2)/(M3*SIN(N4/2))</f>
         <v>0.95979508052393891</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <f>SIN(3*M3*N4/2)/(M3*SIN(3*N4/2))</f>
         <v>0.66666666666666674</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <f>SIN(5*M3*N4/2)/(M3*SIN(5*N4/2))</f>
         <v>0.21756788155537973</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <f>SIN(7*M3*N4/2)/(M3*SIN(7*N4/2))</f>
         <v>-0.17736296207931862</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <f>SIN(9*M3*N4/2)/(M3*SIN(9*N4/2))</f>
         <v>-0.33333333333333331</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="7">
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="6">
         <f>M2/3</f>
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="7">
+      <c r="B4" s="14"/>
+      <c r="C4" s="6">
         <f>M3*M5*C1/2*2</f>
         <v>72</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="J4" s="8" t="s">
+      <c r="D4" s="6"/>
+      <c r="J4" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="7">
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="6">
         <f>180/M2</f>
         <v>20</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="6">
         <f>PI()/(180/M4)</f>
         <v>0.3490658503988659</v>
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="7">
-        <f>(40*C6/M5)/2</f>
-        <v>2.1666666666666665</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="6">
+        <f>(29.7*C6/M5)/2</f>
+        <v>1.6087499999999999</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="7">
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7">
+      <c r="B6" s="14"/>
+      <c r="C6" s="6">
         <v>0.65</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7">
+      <c r="B8" s="14"/>
+      <c r="C8" s="6">
         <v>380</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7">
+      <c r="B9" s="14"/>
+      <c r="C9" s="6">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="6">
+        <f>C8*C9*SQRT(3)</f>
+        <v>6581.7930687617336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="10"/>
+      <c r="AH13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI13" s="10"/>
+      <c r="AJ13" s="10"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="1"/>
+      <c r="AT13" s="1"/>
+      <c r="AU13" s="1"/>
+      <c r="AV13" s="1"/>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="1"/>
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="1"/>
+    </row>
+    <row r="14" spans="1:52" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="7">
-        <f>C8*C9*SQRT(3)</f>
-        <v>13163.586137523467</v>
-      </c>
-    </row>
-    <row r="13" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
-      <c r="AE13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF13" s="1"/>
-      <c r="AG13" s="1"/>
-      <c r="AH13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI13" s="1"/>
-      <c r="AJ13" s="1"/>
-      <c r="AK13" s="2"/>
-      <c r="AL13" s="2"/>
-      <c r="AM13" s="2"/>
-      <c r="AN13" s="2"/>
-      <c r="AO13" s="2"/>
-      <c r="AP13" s="2"/>
-      <c r="AQ13" s="2"/>
-      <c r="AR13" s="2"/>
-      <c r="AS13" s="2"/>
-      <c r="AT13" s="2"/>
-      <c r="AU13" s="2"/>
-      <c r="AV13" s="2"/>
-      <c r="AW13" s="2"/>
-      <c r="AX13" s="2"/>
-      <c r="AY13" s="2"/>
-      <c r="AZ13" s="2"/>
-    </row>
-    <row r="14" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" s="4" t="s">
+      <c r="P14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Q14" s="4" t="s">
+      <c r="Q14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="S14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T14" s="4" t="s">
+      <c r="T14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="U14" s="4" t="s">
+      <c r="U14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V14" s="4" t="s">
+      <c r="V14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="W14" s="4" t="s">
+      <c r="W14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X14" s="4" t="s">
+      <c r="X14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Y14" s="4" t="s">
+      <c r="Y14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Z14" s="4" t="s">
+      <c r="Z14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AA14" s="4" t="s">
+      <c r="AA14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AB14" s="4" t="s">
+      <c r="AB14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AC14" s="4" t="s">
+      <c r="AC14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AD14" s="4" t="s">
+      <c r="AD14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AE14" s="4" t="s">
+      <c r="AE14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AF14" s="4" t="s">
+      <c r="AF14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AG14" s="4" t="s">
+      <c r="AG14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AH14" s="4" t="s">
+      <c r="AH14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AI14" s="4" t="s">
+      <c r="AI14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AJ14" s="4" t="s">
+      <c r="AJ14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AK14" s="2"/>
-      <c r="AL14" s="2"/>
-      <c r="AM14" s="2"/>
-      <c r="AN14" s="2"/>
-      <c r="AO14" s="2"/>
-      <c r="AP14" s="2"/>
-      <c r="AQ14" s="2"/>
-      <c r="AR14" s="2"/>
-      <c r="AS14" s="2"/>
-      <c r="AT14" s="2"/>
-      <c r="AU14" s="2"/>
-      <c r="AV14" s="2"/>
-      <c r="AW14" s="2"/>
-      <c r="AX14" s="2"/>
-      <c r="AY14" s="2"/>
-      <c r="AZ14" s="2"/>
-    </row>
-    <row r="15" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
+      <c r="AS14" s="1"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="1"/>
+      <c r="AV14" s="1"/>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="1"/>
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1"/>
+    </row>
+    <row r="15" spans="1:52" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="N15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="O15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="P15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="Q15" s="4" t="s">
+      <c r="Q15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="S15" s="4" t="s">
+      <c r="S15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="T15" s="4" t="s">
+      <c r="T15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="U15" s="4" t="s">
+      <c r="U15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="V15" s="4" t="s">
+      <c r="V15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="W15" s="4" t="s">
+      <c r="W15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="X15" s="4" t="s">
+      <c r="X15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="Y15" s="4" t="s">
+      <c r="Y15" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="Z15" s="4" t="s">
+      <c r="Z15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AA15" s="4" t="s">
+      <c r="AA15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="AB15" s="4" t="s">
+      <c r="AB15" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AC15" s="4" t="s">
+      <c r="AC15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AD15" s="4" t="s">
+      <c r="AD15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AE15" s="4" t="s">
+      <c r="AE15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AF15" s="4" t="s">
+      <c r="AF15" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AG15" s="4" t="s">
+      <c r="AG15" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AH15" s="4" t="s">
+      <c r="AH15" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AI15" s="4" t="s">
+      <c r="AI15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AJ15" s="4" t="s">
+      <c r="AJ15" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AK15" s="2"/>
-      <c r="AL15" s="2"/>
-      <c r="AM15" s="2"/>
-      <c r="AN15" s="2"/>
-      <c r="AO15" s="2"/>
-      <c r="AP15" s="2"/>
-      <c r="AQ15" s="2"/>
-      <c r="AR15" s="2"/>
-      <c r="AS15" s="2"/>
-      <c r="AT15" s="2"/>
-      <c r="AU15" s="2"/>
-      <c r="AV15" s="2"/>
-      <c r="AW15" s="2"/>
-      <c r="AX15" s="2"/>
-      <c r="AY15" s="2"/>
-      <c r="AZ15" s="2"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <f>-D23</f>
         <v>-0.3490658503988659</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>-1</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <f>E21*-1</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>0</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>1</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <f t="shared" ref="F22:F40" si="0">E22*-1</f>
         <v>-1</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <f>$D$31/9</f>
         <v>0.3490658503988659</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>3</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="5">
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <f>2*$D$31/9</f>
         <v>0.69813170079773179</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>4</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <f>3*$D$31/9</f>
         <v>1.0471975511965976</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>5</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <f>4*$D$31/9</f>
         <v>1.3962634015954636</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>6</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <f t="shared" si="0"/>
         <v>-6</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <f>5*$D$31/9</f>
         <v>1.7453292519943295</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>5</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <f>6*$D$31/9</f>
         <v>2.0943951023931953</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>4</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <f>7*$D$31/9</f>
         <v>2.4434609527920612</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>3</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="5">
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <f>8*$D$31/9</f>
         <v>2.7925268031909272</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>1</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="5">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>-1</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <f>10*$D$31/9</f>
         <v>3.4906585039886591</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>-3</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <f>11*$D$31/9</f>
         <v>3.8397243543875246</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
         <v>-4</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <f>12*$D$31/9</f>
         <v>4.1887902047863905</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="5">
         <v>-5</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <f>13*$D$31/9</f>
         <v>4.5378560551852569</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
         <v>-6</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <f>14*$D$31/9</f>
         <v>4.8869219055841224</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="5">
         <v>-5</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <f>15*$D$31/9</f>
         <v>5.2359877559829879</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="5">
         <v>-4</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D38" s="6">
+      <c r="D38" s="5">
         <f>16*$D$31/9</f>
         <v>5.5850536063818543</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
         <v>-3</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <f>17*$D$31/9</f>
         <v>5.9341194567807207</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
         <v>-1</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <f>18*$D$31/9</f>
         <v>6.2831853071795862</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="5">
         <v>1</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="5">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
     </row>
     <row r="61" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" s="12"/>
-    </row>
-    <row r="64" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+      <c r="A61" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="8"/>
+    </row>
+    <row r="64" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="1" t="s">
+      <c r="B64" s="12"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1" t="s">
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1" t="s">
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1" t="s">
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
+      <c r="M64" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
-      <c r="P64" s="1" t="s">
+      <c r="N64" s="10"/>
+      <c r="O64" s="10"/>
+      <c r="P64" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
-      <c r="S64" s="1" t="s">
+      <c r="Q64" s="10"/>
+      <c r="R64" s="10"/>
+      <c r="S64" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="T64" s="1"/>
-      <c r="U64" s="1"/>
-      <c r="V64" s="1" t="s">
+      <c r="T64" s="10"/>
+      <c r="U64" s="10"/>
+      <c r="V64" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="W64" s="1"/>
-      <c r="X64" s="1"/>
-      <c r="Y64" s="1" t="s">
+      <c r="W64" s="10"/>
+      <c r="X64" s="10"/>
+      <c r="Y64" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="Z64" s="1"/>
-      <c r="AA64" s="1"/>
-      <c r="AB64" s="1" t="s">
+      <c r="Z64" s="10"/>
+      <c r="AA64" s="10"/>
+      <c r="AB64" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AC64" s="1"/>
-      <c r="AD64" s="1"/>
-      <c r="AE64" s="1" t="s">
+      <c r="AC64" s="10"/>
+      <c r="AD64" s="10"/>
+      <c r="AE64" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="AF64" s="1"/>
-      <c r="AG64" s="1"/>
-      <c r="AH64" s="1" t="s">
+      <c r="AF64" s="10"/>
+      <c r="AG64" s="10"/>
+      <c r="AH64" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AI64" s="1"/>
-      <c r="AJ64" s="1"/>
-      <c r="AK64" s="2"/>
-      <c r="AL64" s="2"/>
-      <c r="AM64" s="2"/>
-      <c r="AN64" s="2"/>
-      <c r="AO64" s="2"/>
-      <c r="AP64" s="2"/>
-      <c r="AQ64" s="2"/>
-      <c r="AR64" s="2"/>
-      <c r="AS64" s="2"/>
-      <c r="AT64" s="2"/>
-      <c r="AU64" s="2"/>
-      <c r="AV64" s="2"/>
-      <c r="AW64" s="2"/>
-      <c r="AX64" s="2"/>
-      <c r="AY64" s="2"/>
-      <c r="AZ64" s="2"/>
-    </row>
-    <row r="65" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="AI64" s="10"/>
+      <c r="AJ64" s="10"/>
+      <c r="AK64" s="1"/>
+      <c r="AL64" s="1"/>
+      <c r="AM64" s="1"/>
+      <c r="AN64" s="1"/>
+      <c r="AO64" s="1"/>
+      <c r="AP64" s="1"/>
+      <c r="AQ64" s="1"/>
+      <c r="AR64" s="1"/>
+      <c r="AS64" s="1"/>
+      <c r="AT64" s="1"/>
+      <c r="AU64" s="1"/>
+      <c r="AV64" s="1"/>
+      <c r="AW64" s="1"/>
+      <c r="AX64" s="1"/>
+      <c r="AY64" s="1"/>
+      <c r="AZ64" s="1"/>
+    </row>
+    <row r="65" spans="1:52" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G65" s="4" t="s">
+      <c r="G65" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H65" s="4" t="s">
+      <c r="H65" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I65" s="4" t="s">
+      <c r="I65" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J65" s="4" t="s">
+      <c r="J65" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K65" s="4" t="s">
+      <c r="K65" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L65" s="4" t="s">
+      <c r="L65" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M65" s="4" t="s">
+      <c r="M65" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N65" s="4" t="s">
+      <c r="N65" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O65" s="4" t="s">
+      <c r="O65" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P65" s="4" t="s">
+      <c r="P65" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Q65" s="4" t="s">
+      <c r="Q65" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R65" s="4" t="s">
+      <c r="R65" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="S65" s="4" t="s">
+      <c r="S65" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T65" s="4" t="s">
+      <c r="T65" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="U65" s="4" t="s">
+      <c r="U65" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="V65" s="4" t="s">
+      <c r="V65" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="W65" s="4" t="s">
+      <c r="W65" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X65" s="4" t="s">
+      <c r="X65" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Y65" s="4" t="s">
+      <c r="Y65" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Z65" s="4" t="s">
+      <c r="Z65" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AA65" s="4" t="s">
+      <c r="AA65" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AB65" s="4" t="s">
+      <c r="AB65" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AC65" s="4" t="s">
+      <c r="AC65" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AD65" s="4" t="s">
+      <c r="AD65" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AE65" s="4" t="s">
+      <c r="AE65" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AF65" s="4" t="s">
+      <c r="AF65" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AG65" s="4" t="s">
+      <c r="AG65" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AH65" s="4" t="s">
+      <c r="AH65" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AI65" s="4" t="s">
+      <c r="AI65" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AJ65" s="4" t="s">
+      <c r="AJ65" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AK65" s="2"/>
-      <c r="AL65" s="2"/>
-      <c r="AM65" s="2"/>
-      <c r="AN65" s="2"/>
-      <c r="AO65" s="2"/>
-      <c r="AP65" s="2"/>
-      <c r="AQ65" s="2"/>
-      <c r="AR65" s="2"/>
-      <c r="AS65" s="2"/>
-      <c r="AT65" s="2"/>
-      <c r="AU65" s="2"/>
-      <c r="AV65" s="2"/>
-      <c r="AW65" s="2"/>
-      <c r="AX65" s="2"/>
-      <c r="AY65" s="2"/>
-      <c r="AZ65" s="2"/>
-    </row>
-    <row r="66" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+      <c r="AK65" s="1"/>
+      <c r="AL65" s="1"/>
+      <c r="AM65" s="1"/>
+      <c r="AN65" s="1"/>
+      <c r="AO65" s="1"/>
+      <c r="AP65" s="1"/>
+      <c r="AQ65" s="1"/>
+      <c r="AR65" s="1"/>
+      <c r="AS65" s="1"/>
+      <c r="AT65" s="1"/>
+      <c r="AU65" s="1"/>
+      <c r="AV65" s="1"/>
+      <c r="AW65" s="1"/>
+      <c r="AX65" s="1"/>
+      <c r="AY65" s="1"/>
+      <c r="AZ65" s="1"/>
+    </row>
+    <row r="66" spans="1:52" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E66" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="F66" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G66" s="4" t="s">
+      <c r="G66" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H66" s="4" t="s">
+      <c r="H66" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I66" s="4" t="s">
+      <c r="I66" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J66" s="4" t="s">
+      <c r="J66" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K66" s="4" t="s">
+      <c r="K66" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L66" s="4" t="s">
+      <c r="L66" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="M66" s="4" t="s">
+      <c r="M66" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="N66" s="4" t="s">
+      <c r="N66" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="O66" s="4" t="s">
+      <c r="O66" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P66" s="4" t="s">
+      <c r="P66" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Q66" s="4" t="s">
+      <c r="Q66" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="R66" s="4" t="s">
+      <c r="R66" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="S66" s="4" t="s">
+      <c r="S66" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T66" s="4" t="s">
+      <c r="T66" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="U66" s="4" t="s">
+      <c r="U66" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="V66" s="4" t="s">
+      <c r="V66" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="W66" s="4" t="s">
+      <c r="W66" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="X66" s="4" t="s">
+      <c r="X66" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="Y66" s="4" t="s">
+      <c r="Y66" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="Z66" s="4" t="s">
+      <c r="Z66" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AA66" s="4" t="s">
+      <c r="AA66" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AB66" s="4" t="s">
+      <c r="AB66" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AC66" s="4" t="s">
+      <c r="AC66" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AD66" s="4" t="s">
+      <c r="AD66" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AE66" s="4" t="s">
+      <c r="AE66" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AF66" s="4" t="s">
+      <c r="AF66" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AG66" s="4" t="s">
+      <c r="AG66" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AH66" s="4" t="s">
+      <c r="AH66" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AI66" s="4" t="s">
+      <c r="AI66" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AJ66" s="4" t="s">
+      <c r="AJ66" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AK66" s="2"/>
-      <c r="AL66" s="2"/>
-      <c r="AM66" s="2"/>
-      <c r="AN66" s="2"/>
-      <c r="AO66" s="2"/>
-      <c r="AP66" s="2"/>
-      <c r="AQ66" s="2"/>
-      <c r="AR66" s="2"/>
-      <c r="AS66" s="2"/>
-      <c r="AT66" s="2"/>
-      <c r="AU66" s="2"/>
-      <c r="AV66" s="2"/>
-      <c r="AW66" s="2"/>
-      <c r="AX66" s="2"/>
-      <c r="AY66" s="2"/>
-      <c r="AZ66" s="2"/>
+      <c r="AK66" s="1"/>
+      <c r="AL66" s="1"/>
+      <c r="AM66" s="1"/>
+      <c r="AN66" s="1"/>
+      <c r="AO66" s="1"/>
+      <c r="AP66" s="1"/>
+      <c r="AQ66" s="1"/>
+      <c r="AR66" s="1"/>
+      <c r="AS66" s="1"/>
+      <c r="AT66" s="1"/>
+      <c r="AU66" s="1"/>
+      <c r="AV66" s="1"/>
+      <c r="AW66" s="1"/>
+      <c r="AX66" s="1"/>
+      <c r="AY66" s="1"/>
+      <c r="AZ66" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="S64:U64"/>
-    <mergeCell ref="V64:X64"/>
-    <mergeCell ref="Y64:AA64"/>
-    <mergeCell ref="AB64:AD64"/>
-    <mergeCell ref="AE64:AG64"/>
+    <mergeCell ref="AH13:AJ13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="AB13:AD13"/>
+    <mergeCell ref="AE13:AG13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J5:L5"/>
     <mergeCell ref="AH64:AJ64"/>
     <mergeCell ref="A64:C64"/>
     <mergeCell ref="D64:F64"/>
@@ -3443,36 +3406,115 @@
     <mergeCell ref="J64:L64"/>
     <mergeCell ref="M64:O64"/>
     <mergeCell ref="P64:R64"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="Y13:AA13"/>
-    <mergeCell ref="AB13:AD13"/>
-    <mergeCell ref="AE13:AG13"/>
-    <mergeCell ref="AH13:AJ13"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="S64:U64"/>
+    <mergeCell ref="V64:X64"/>
+    <mergeCell ref="Y64:AA64"/>
+    <mergeCell ref="AB64:AD64"/>
+    <mergeCell ref="AE64:AG64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="7"/>
+    <col min="5" max="5" width="33.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <f>(B2/(0.135*'Winding Design'!C1))^2</f>
+        <v>8.5733882030178312E-3</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="C2" s="7">
+        <v>29.7</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.48</v>
+      </c>
+      <c r="E2" s="7">
+        <v>26000</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="H2" s="7">
+        <f>(120*50/'Winding Design'!C1)/60</f>
+        <v>25</v>
+      </c>
+      <c r="I2" s="7">
+        <f>('Winding Design'!C10/1000)/(J2*H2)</f>
+        <v>12283.205496645896</v>
+      </c>
+      <c r="J2" s="7">
+        <f>B2^2*K2</f>
+        <v>2.1433470507544583E-5</v>
+      </c>
+      <c r="K2" s="7">
+        <f>(B2/(0.135*'Winding Design'!C1))^2</f>
+        <v>8.5733882030178312E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Design parameters are updated, analytical calculations are completed.
</commit_message>
<xml_diff>
--- a/Project 2/Winding Design.xlsx
+++ b/Project 2/Winding Design.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="127">
   <si>
     <t>A</t>
   </si>
@@ -292,9 +292,6 @@
     <t>Conductors per Slot</t>
   </si>
   <si>
-    <t>Wye</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt; </t>
   </si>
   <si>
@@ -316,18 +313,9 @@
     <t>coil span=120 (6 slots)</t>
   </si>
   <si>
-    <t>Axial Length (mm)</t>
-  </si>
-  <si>
     <t>16AWG</t>
   </si>
   <si>
-    <t>A (mm)</t>
-  </si>
-  <si>
-    <t>Bavg(T)</t>
-  </si>
-  <si>
     <t>Specific Electric Loading-q (A/m)</t>
   </si>
   <si>
@@ -350,6 +338,69 @@
   </si>
   <si>
     <t>Di (m)</t>
+  </si>
+  <si>
+    <t>Nphase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Flux per Pole (Wb)</t>
+  </si>
+  <si>
+    <t>Bavg (T)</t>
+  </si>
+  <si>
+    <t>Axial Length (m)</t>
+  </si>
+  <si>
+    <t>Airgap Clearance (m)</t>
+  </si>
+  <si>
+    <t>A (mm^2)</t>
+  </si>
+  <si>
+    <t>Specific Magnetic Loading (T)</t>
+  </si>
+  <si>
+    <t>Flux Density in Teeth (T)</t>
+  </si>
+  <si>
+    <t>Flux Density in Core (T)</t>
+  </si>
+  <si>
+    <t>Torque (N.m)</t>
+  </si>
+  <si>
+    <t>Speed (rad/s)</t>
+  </si>
+  <si>
+    <t>Pole Pitch (m)</t>
+  </si>
+  <si>
+    <t>l_mt (m)</t>
+  </si>
+  <si>
+    <t>Phase Resistance (ohm)</t>
+  </si>
+  <si>
+    <t>Copper Losses (W)</t>
+  </si>
+  <si>
+    <t>wye</t>
+  </si>
+  <si>
+    <t>Phase Inductance</t>
+  </si>
+  <si>
+    <t>Core Mass (kg)</t>
+  </si>
+  <si>
+    <t>Core Loss (W)</t>
+  </si>
+  <si>
+    <t>Do (m)</t>
   </si>
 </sst>
 </file>
@@ -463,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -482,6 +533,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -497,6 +551,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2262,7 +2317,7 @@
   <dimension ref="A1:AZ66"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,47 +2328,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="15"/>
       <c r="C1" s="6">
         <v>4</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
       <c r="M1" s="6">
         <v>36</v>
       </c>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q1" s="10">
+        <f>'Motor Parameter Estimation'!B2</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
       <c r="M2" s="6">
         <f>M1/C1</f>
         <v>9</v>
       </c>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q2" s="10">
+        <f>'Motor Parameter Estimation'!A2</f>
+        <v>5.3583676268861444E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="6">
         <f>SIN(M3*N4/2)/(M3*SIN(N4/2))</f>
         <v>0.95979508052393891</v>
@@ -2334,304 +2405,281 @@
         <f>SIN(9*M3*N4/2)/(M3*SIN(9*N4/2))</f>
         <v>-0.33333333333333331</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
       <c r="M3" s="6">
         <f>M2/3</f>
         <v>3</v>
       </c>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="6">
         <f>M3*M5*C1/2*2</f>
-        <v>72</v>
+        <v>240</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
       <c r="M4" s="6">
         <f>180/M2</f>
         <v>20</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="10">
         <f>PI()/(180/M4)</f>
         <v>0.3490658503988659</v>
       </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="14"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="6">
+        <f>(107.5*C6/M5)/2</f>
+        <v>1.34375</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="6">
-        <f>(29.7*C6/M5)/2</f>
-        <v>1.6087499999999999</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="J5" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="6">
+        <v>20</v>
+      </c>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="J6" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="9">
+        <f>(M3*M5*C1/2)*2</f>
+        <v>240</v>
+      </c>
+      <c r="N6" s="10">
+        <f>(C8/SQRT(3))/(4.44*C11*C3*N7)</f>
+        <v>244.66344551356454</v>
+      </c>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="J7" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="16">
+        <f>(C8/SQRT(3))/(4.44*C11*C3*M6)</f>
+        <v>4.2902266222646698E-3</v>
+      </c>
+      <c r="N7" s="10">
+        <f>M8*PI()*Q1*Q2/C1</f>
+        <v>4.2084520929647215E-3</v>
+      </c>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="J5" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="6">
-        <v>0.65</v>
-      </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="14"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="6">
         <v>380</v>
       </c>
       <c r="D8" s="6"/>
+      <c r="J8" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="6">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="J9" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="6">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="14"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="6">
         <f>C8*C9*SQRT(3)</f>
         <v>6581.7930687617336</v>
       </c>
-    </row>
-    <row r="13" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="J10" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="10">
+        <f>(0.5*M8^2*PI()*Q1^2*Q2/2)/(4*PI()*10^-7)</f>
+        <v>334.89797668038403</v>
+      </c>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="10">
+        <v>50</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="10">
+        <f>C10/M10</f>
+        <v>19.653128794633439</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="14" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="10" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10" t="s">
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10" t="s">
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10" t="s">
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10" t="s">
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10" t="s">
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="10" t="s">
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Z13" s="10"/>
-      <c r="AA13" s="10"/>
-      <c r="AB13" s="10" t="s">
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="AC13" s="10"/>
-      <c r="AD13" s="10"/>
-      <c r="AE13" s="10" t="s">
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AF13" s="10"/>
-      <c r="AG13" s="10"/>
-      <c r="AH13" s="10" t="s">
+      <c r="AF14" s="11"/>
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AI13" s="10"/>
-      <c r="AJ13" s="10"/>
-      <c r="AK13" s="1"/>
-      <c r="AL13" s="1"/>
-      <c r="AM13" s="1"/>
-      <c r="AN13" s="1"/>
-      <c r="AO13" s="1"/>
-      <c r="AP13" s="1"/>
-      <c r="AQ13" s="1"/>
-      <c r="AR13" s="1"/>
-      <c r="AS13" s="1"/>
-      <c r="AT13" s="1"/>
-      <c r="AU13" s="1"/>
-      <c r="AV13" s="1"/>
-      <c r="AW13" s="1"/>
-      <c r="AX13" s="1"/>
-      <c r="AY13" s="1"/>
-      <c r="AZ13" s="1"/>
-    </row>
-    <row r="14" spans="1:52" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="W14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="X14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ14" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="11"/>
       <c r="AK14" s="1"/>
       <c r="AL14" s="1"/>
       <c r="AM14" s="1"/>
@@ -2651,112 +2699,112 @@
     </row>
     <row r="15" spans="1:52" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="V15" s="3" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="X15" s="3" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="Y15" s="3" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="AA15" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="AB15" s="3" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="AC15" s="3" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="AD15" s="3" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="AE15" s="3" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="AF15" s="3" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="AG15" s="3" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="AH15" s="3" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="AI15" s="3" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="AJ15" s="3" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="AK15" s="1"/>
       <c r="AL15" s="1"/>
@@ -2775,6 +2823,132 @@
       <c r="AY15" s="1"/>
       <c r="AZ15" s="1"/>
     </row>
+    <row r="16" spans="1:52" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="1"/>
+    </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21" s="5">
         <f>-D23</f>
@@ -3036,71 +3210,71 @@
     </row>
     <row r="61" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B61" s="8"/>
     </row>
     <row r="64" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="10" t="s">
+      <c r="B64" s="13"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10" t="s">
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10" t="s">
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K64" s="10"/>
-      <c r="L64" s="10"/>
-      <c r="M64" s="10" t="s">
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="N64" s="10"/>
-      <c r="O64" s="10"/>
-      <c r="P64" s="10" t="s">
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Q64" s="10"/>
-      <c r="R64" s="10"/>
-      <c r="S64" s="10" t="s">
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="T64" s="10"/>
-      <c r="U64" s="10"/>
-      <c r="V64" s="10" t="s">
+      <c r="T64" s="11"/>
+      <c r="U64" s="11"/>
+      <c r="V64" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="W64" s="10"/>
-      <c r="X64" s="10"/>
-      <c r="Y64" s="10" t="s">
+      <c r="W64" s="11"/>
+      <c r="X64" s="11"/>
+      <c r="Y64" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Z64" s="10"/>
-      <c r="AA64" s="10"/>
-      <c r="AB64" s="10" t="s">
+      <c r="Z64" s="11"/>
+      <c r="AA64" s="11"/>
+      <c r="AB64" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="AC64" s="10"/>
-      <c r="AD64" s="10"/>
-      <c r="AE64" s="10" t="s">
+      <c r="AC64" s="11"/>
+      <c r="AD64" s="11"/>
+      <c r="AE64" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AF64" s="10"/>
-      <c r="AG64" s="10"/>
-      <c r="AH64" s="10" t="s">
+      <c r="AF64" s="11"/>
+      <c r="AG64" s="11"/>
+      <c r="AH64" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AI64" s="10"/>
-      <c r="AJ64" s="10"/>
+      <c r="AI64" s="11"/>
+      <c r="AJ64" s="11"/>
       <c r="AK64" s="1"/>
       <c r="AL64" s="1"/>
       <c r="AM64" s="1"/>
@@ -3371,19 +3545,27 @@
       <c r="AZ66" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="AH13:AJ13"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="Y13:AA13"/>
-    <mergeCell ref="AB13:AD13"/>
-    <mergeCell ref="AE13:AG13"/>
+  <mergeCells count="47">
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="AH14:AJ14"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="Y14:AA14"/>
+    <mergeCell ref="AB14:AD14"/>
+    <mergeCell ref="AE14:AG14"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A10:B10"/>
@@ -3420,97 +3602,163 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="7"/>
-    <col min="5" max="5" width="33.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="7"/>
+    <col min="2" max="2" width="9.140625" style="7"/>
+    <col min="3" max="3" width="25" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.5703125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="I1" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="K1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>(B2/(0.135*'Winding Design'!C1))^2</f>
-        <v>8.5733882030178312E-3</v>
+        <v>5.3583676268861444E-2</v>
       </c>
       <c r="B2" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="C2" s="7">
-        <v>29.7</v>
+        <v>0.125</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.2</v>
       </c>
       <c r="D2" s="7">
-        <v>0.48</v>
+        <v>107.5</v>
       </c>
       <c r="E2" s="7">
-        <v>26000</v>
-      </c>
-      <c r="F2" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="H2" s="7">
+        <f>L2/(11*E2*'Winding Design'!C3*I2*J2*10^-3)</f>
+        <v>41366.424250200864</v>
+      </c>
+      <c r="I2" s="7">
         <v>0.9</v>
       </c>
-      <c r="G2" s="7">
+      <c r="J2" s="7">
         <v>0.9</v>
       </c>
-      <c r="H2" s="7">
+      <c r="K2" s="7">
         <f>(120*50/'Winding Design'!C1)/60</f>
         <v>25</v>
       </c>
-      <c r="I2" s="7">
-        <f>('Winding Design'!C10/1000)/(J2*H2)</f>
-        <v>12283.205496645896</v>
-      </c>
-      <c r="J2" s="7">
-        <f>B2^2*K2</f>
-        <v>2.1433470507544583E-5</v>
-      </c>
-      <c r="K2" s="7">
-        <f>(B2/(0.135*'Winding Design'!C1))^2</f>
-        <v>8.5733882030178312E-3</v>
+      <c r="L2" s="7">
+        <f>(('Winding Design'!C10*0.9)/(K2*M2))/1000</f>
+        <v>283.00505464272152</v>
+      </c>
+      <c r="M2" s="7">
+        <f>B2^2*A2</f>
+        <v>8.3724494170096006E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <f>PI()*B2/'Winding Design'!C1</f>
+        <v>9.8174770424681035E-2</v>
+      </c>
+      <c r="B5" s="7">
+        <f>2*A2+2.3*A5+0.24</f>
+        <v>0.57296932451448923</v>
+      </c>
+      <c r="C5" s="7">
+        <f>0.021*B5*'Winding Design'!M6/1.31</f>
+        <v>2.2044010653076533</v>
+      </c>
+      <c r="D5" s="7">
+        <f>3*'Winding Design'!C9^2*C5</f>
+        <v>661.32031959229596</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10">
+        <f>PI()*(C2/2)^2*A2*7850</f>
+        <v>13.214539571909226</v>
+      </c>
+      <c r="G5" s="7">
+        <f>F5*0.95</f>
+        <v>12.553812593313765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Design is optimized, RMXPRT tool is used for verification and all relevant data is obtained.
</commit_message>
<xml_diff>
--- a/Project 2/Winding Design.xlsx
+++ b/Project 2/Winding Design.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="132">
   <si>
     <t>A</t>
   </si>
@@ -304,18 +304,12 @@
     <t>Current Rating (A)</t>
   </si>
   <si>
-    <t>Power Rating (W)</t>
-  </si>
-  <si>
     <t>Integral, Double Layer, Distributed Winding</t>
   </si>
   <si>
     <t>coil span=120 (6 slots)</t>
   </si>
   <si>
-    <t>16AWG</t>
-  </si>
-  <si>
     <t>Specific Electric Loading-q (A/m)</t>
   </si>
   <si>
@@ -385,15 +379,9 @@
     <t>Phase Resistance (ohm)</t>
   </si>
   <si>
-    <t>Copper Losses (W)</t>
-  </si>
-  <si>
     <t>wye</t>
   </si>
   <si>
-    <t>Phase Inductance</t>
-  </si>
-  <si>
     <t>Core Mass (kg)</t>
   </si>
   <si>
@@ -401,6 +389,33 @@
   </si>
   <si>
     <t>Do (m)</t>
+  </si>
+  <si>
+    <t>Phase Inductance (mH)</t>
+  </si>
+  <si>
+    <t>Leakage Inductance (mH)</t>
+  </si>
+  <si>
+    <t>rpm</t>
+  </si>
+  <si>
+    <t>14AWG</t>
+  </si>
+  <si>
+    <t>(17AWG-1,04mm^2)</t>
+  </si>
+  <si>
+    <t>Output Power Rating (W)</t>
+  </si>
+  <si>
+    <t>Input Power Rating (W)</t>
+  </si>
+  <si>
+    <t>Stator Copper Losses (W)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -514,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -536,6 +551,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -551,7 +570,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1957,7 +1975,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>376518</xdr:colOff>
+      <xdr:colOff>5043</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>138113</xdr:rowOff>
     </xdr:to>
@@ -2006,8 +2024,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>99</xdr:row>
       <xdr:rowOff>96648</xdr:rowOff>
     </xdr:to>
@@ -2317,74 +2335,76 @@
   <dimension ref="A1:AZ66"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="14.7109375" style="5" customWidth="1"/>
+    <col min="3" max="6" width="9.140625" style="5"/>
     <col min="7" max="7" width="9.140625" style="5" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="6">
         <v>4</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
       <c r="M1" s="6">
         <v>36</v>
       </c>
       <c r="O1" s="10"/>
       <c r="P1" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q1" s="10">
         <f>'Motor Parameter Estimation'!B2</f>
-        <v>0.125</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
       <c r="M2" s="6">
         <f>M1/C1</f>
         <v>9</v>
       </c>
       <c r="O2" s="10"/>
       <c r="P2" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q2" s="10">
         <f>'Motor Parameter Estimation'!A2</f>
-        <v>5.3583676268861444E-2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="6">
         <f>SIN(M3*N4/2)/(M3*SIN(N4/2))</f>
         <v>0.95979508052393891</v>
@@ -2405,11 +2425,11 @@
         <f>SIN(9*M3*N4/2)/(M3*SIN(9*N4/2))</f>
         <v>-0.33333333333333331</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
       <c r="M3" s="6">
         <f>M2/3</f>
         <v>3</v>
@@ -2419,20 +2439,20 @@
       <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="6">
-        <f>M3*M5*C1/2*2</f>
-        <v>240</v>
+        <f>M3*M5*C1/2</f>
+        <v>180</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
       <c r="M4" s="6">
         <f>180/M2</f>
         <v>20</v>
@@ -2446,30 +2466,30 @@
       <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="6" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>90</v>
       </c>
       <c r="E5" s="6">
-        <f>(107.5*C6/M5)/2</f>
-        <v>1.34375</v>
+        <f>('Motor Parameter Estimation'!D2*C6/M5)</f>
+        <v>2.1769999999999996</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
       <c r="M5" s="6">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
@@ -2477,94 +2497,96 @@
       <c r="Q5" s="10"/>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="6">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="J6" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
+      <c r="J6" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
       <c r="M6" s="9">
-        <f>(M3*M5*C1/2)*2</f>
-        <v>240</v>
+        <f>(M3*M5*C1/2)</f>
+        <v>180</v>
       </c>
       <c r="N6" s="10">
         <f>(C8/SQRT(3))/(4.44*C11*C3*N7)</f>
-        <v>244.66344551356454</v>
+        <v>71.249819887081856</v>
       </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="J7" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="16">
+      <c r="J7" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="11">
         <f>(C8/SQRT(3))/(4.44*C11*C3*M6)</f>
-        <v>4.2902266222646698E-3</v>
+        <v>5.7203021630195597E-3</v>
       </c>
       <c r="N7" s="10">
-        <f>M8*PI()*Q1*Q2/C1</f>
-        <v>4.2084520929647215E-3</v>
+        <f>N8*PI()*Q1*Q2/C1</f>
+        <v>1.445132620651305E-2</v>
       </c>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="6">
         <v>380</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="J8" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="10">
+      <c r="J8" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="9">
+        <f>M7/(PI()*Q1*Q2/C1)</f>
+        <v>0.3166658661648083</v>
+      </c>
+      <c r="N8" s="10">
         <v>0.8</v>
       </c>
-      <c r="N8" s="10"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="6">
-        <f>10</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="J9" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="J9" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
       <c r="M9" s="10">
         <v>1E-3</v>
       </c>
@@ -2574,112 +2596,139 @@
       <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" s="15"/>
+      <c r="A10" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="17"/>
       <c r="C10" s="6">
-        <f>C8*C9*SQRT(3)</f>
-        <v>6581.7930687617336</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="10">
+        <v>3000</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="11">
+        <f>C10/M12</f>
+        <v>20.462778397529405</v>
+      </c>
+      <c r="N10" s="10">
         <f>(0.5*M8^2*PI()*Q1^2*Q2/2)/(4*PI()*10^-7)</f>
-        <v>334.89797668038403</v>
+        <v>165.7708632811796</v>
       </c>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="15"/>
+      <c r="A11" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="17"/>
       <c r="C11" s="10">
         <v>50</v>
       </c>
-      <c r="J11" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="J11" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
       <c r="M11" s="10">
-        <f>C10/M10</f>
-        <v>19.653128794633439</v>
+        <f>C10/N10</f>
+        <v>18.09726957210458</v>
+      </c>
+      <c r="N11" s="5">
+        <f>M11*60/(2*PI())</f>
+        <v>172.81619453201964</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="10"/>
+      <c r="A12" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="5">
+        <f>C10/'Motor Parameter Estimation'!I2</f>
+        <v>3871.7081964643635</v>
+      </c>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="9">
+        <f>2*PI()*N12/60</f>
+        <v>146.60765716752366</v>
+      </c>
+      <c r="N12" s="9">
+        <v>1400</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="11" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11" t="s">
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11" t="s">
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11" t="s">
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11" t="s">
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11" t="s">
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11" t="s">
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11" t="s">
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11" t="s">
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
-      <c r="AE14" s="11" t="s">
+      <c r="AC14" s="13"/>
+      <c r="AD14" s="13"/>
+      <c r="AE14" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="AF14" s="11"/>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="11" t="s">
+      <c r="AF14" s="13"/>
+      <c r="AG14" s="13"/>
+      <c r="AH14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="11"/>
+      <c r="AI14" s="13"/>
+      <c r="AJ14" s="13"/>
       <c r="AK14" s="1"/>
       <c r="AL14" s="1"/>
       <c r="AM14" s="1"/>
@@ -3210,71 +3259,71 @@
     </row>
     <row r="61" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B61" s="8"/>
     </row>
     <row r="64" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="13"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="11" t="s">
+      <c r="B64" s="15"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11" t="s">
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11" t="s">
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K64" s="11"/>
-      <c r="L64" s="11"/>
-      <c r="M64" s="11" t="s">
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
+      <c r="M64" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N64" s="11"/>
-      <c r="O64" s="11"/>
-      <c r="P64" s="11" t="s">
+      <c r="N64" s="13"/>
+      <c r="O64" s="13"/>
+      <c r="P64" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="Q64" s="11"/>
-      <c r="R64" s="11"/>
-      <c r="S64" s="11" t="s">
+      <c r="Q64" s="13"/>
+      <c r="R64" s="13"/>
+      <c r="S64" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="T64" s="11"/>
-      <c r="U64" s="11"/>
-      <c r="V64" s="11" t="s">
+      <c r="T64" s="13"/>
+      <c r="U64" s="13"/>
+      <c r="V64" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="W64" s="11"/>
-      <c r="X64" s="11"/>
-      <c r="Y64" s="11" t="s">
+      <c r="W64" s="13"/>
+      <c r="X64" s="13"/>
+      <c r="Y64" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="Z64" s="11"/>
-      <c r="AA64" s="11"/>
-      <c r="AB64" s="11" t="s">
+      <c r="Z64" s="13"/>
+      <c r="AA64" s="13"/>
+      <c r="AB64" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="AC64" s="11"/>
-      <c r="AD64" s="11"/>
-      <c r="AE64" s="11" t="s">
+      <c r="AC64" s="13"/>
+      <c r="AD64" s="13"/>
+      <c r="AE64" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="AF64" s="11"/>
-      <c r="AG64" s="11"/>
-      <c r="AH64" s="11" t="s">
+      <c r="AF64" s="13"/>
+      <c r="AG64" s="13"/>
+      <c r="AH64" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="AI64" s="11"/>
-      <c r="AJ64" s="11"/>
+      <c r="AI64" s="13"/>
+      <c r="AJ64" s="13"/>
       <c r="AK64" s="1"/>
       <c r="AL64" s="1"/>
       <c r="AM64" s="1"/>
@@ -3545,7 +3594,7 @@
       <c r="AZ66" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="48">
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="J7:L7"/>
@@ -3554,6 +3603,7 @@
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="J11:L11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="AH14:AJ14"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="D14:F14"/>
@@ -3602,10 +3652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3613,7 +3663,7 @@
     <col min="1" max="1" width="19.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="7"/>
     <col min="3" max="3" width="25" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="30.5703125" style="10" customWidth="1"/>
     <col min="8" max="8" width="33.5703125" style="7" bestFit="1" customWidth="1"/>
@@ -3626,61 +3676,61 @@
   <sheetData>
     <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>115</v>
-      </c>
       <c r="H1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
-        <f>(B2/(0.135*'Winding Design'!C1))^2</f>
-        <v>5.3583676268861444E-2</v>
+        <v>0.2</v>
       </c>
       <c r="B2" s="7">
-        <v>0.125</v>
+        <v>0.115</v>
       </c>
       <c r="C2" s="10">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="D2" s="7">
-        <v>107.5</v>
+        <v>93.3</v>
       </c>
       <c r="E2" s="7">
-        <v>0.8</v>
+        <f>'Winding Design'!M8</f>
+        <v>0.3166658661648083</v>
       </c>
       <c r="F2" s="10">
         <v>1.5</v>
@@ -3690,39 +3740,40 @@
       </c>
       <c r="H2" s="7">
         <f>L2/(11*E2*'Winding Design'!C3*I2*J2*10^-3)</f>
-        <v>41366.424250200864</v>
+        <v>16962.627505543849</v>
       </c>
       <c r="I2" s="7">
-        <v>0.9</v>
+        <f>('Winding Design'!C10-(H5+D5+50))/'Winding Design'!C10</f>
+        <v>0.77485178318438208</v>
       </c>
       <c r="J2" s="7">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="K2" s="7">
         <f>(120*50/'Winding Design'!C1)/60</f>
         <v>25</v>
       </c>
       <c r="L2" s="7">
-        <f>(('Winding Design'!C10*0.9)/(K2*M2))/1000</f>
-        <v>283.00505464272152</v>
+        <f>(('Winding Design'!C10*I2)/(K2*M2))/1000</f>
+        <v>35.153956136909585</v>
       </c>
       <c r="M2" s="7">
         <f>B2^2*A2</f>
-        <v>8.3724494170096006E-4</v>
+        <v>2.6450000000000002E-3</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>120</v>
-      </c>
       <c r="D4" s="9" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>123</v>
@@ -3731,34 +3782,48 @@
         <v>124</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>PI()*B2/'Winding Design'!C1</f>
-        <v>9.8174770424681035E-2</v>
+        <v>9.0320788790706555E-2</v>
       </c>
       <c r="B5" s="7">
         <f>2*A2+2.3*A5+0.24</f>
-        <v>0.57296932451448923</v>
+        <v>0.84773781421862504</v>
       </c>
       <c r="C5" s="7">
-        <f>0.021*B5*'Winding Design'!M6/1.31</f>
-        <v>2.2044010653076533</v>
+        <f>0.021*B5*'Winding Design'!M6/1.04</f>
+        <v>3.0812009016792334</v>
       </c>
       <c r="D5" s="7">
         <f>3*'Winding Design'!C9^2*C5</f>
-        <v>661.32031959229596</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10">
+        <v>591.59057312241282</v>
+      </c>
+      <c r="E5" s="10">
+        <f>(('Winding Design'!M6^2)/('Winding Design'!M9/((2.5/1000)*A2*4*PI()*10^-7)))/10^-3</f>
+        <v>20.357520395261858</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" s="10">
         <f>PI()*(C2/2)^2*A2*7850</f>
-        <v>13.214539571909226</v>
-      </c>
-      <c r="G5" s="7">
-        <f>F5*0.95</f>
-        <v>12.553812593313765</v>
+        <v>35.635870867832431</v>
+      </c>
+      <c r="H5" s="7">
+        <f>G5*0.95</f>
+        <v>33.854077324440809</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C6" s="10" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All calculation and design is optimized again, reports is concluded.
</commit_message>
<xml_diff>
--- a/Project 2/Winding Design.xlsx
+++ b/Project 2/Winding Design.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="132">
   <si>
     <t>A</t>
   </si>
@@ -529,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -541,9 +541,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -551,7 +548,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,9 +566,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1975,7 +1972,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>5043</xdr:colOff>
+      <xdr:colOff>63475</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>138113</xdr:rowOff>
     </xdr:to>
@@ -2006,8 +2003,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="619125" y="3262313"/>
-          <a:ext cx="10282518" cy="7543800"/>
+          <a:off x="612321" y="3262313"/>
+          <a:ext cx="10259147" cy="7543800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2025,7 +2022,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>601357</xdr:colOff>
       <xdr:row>99</xdr:row>
       <xdr:rowOff>96648</xdr:rowOff>
     </xdr:to>
@@ -2335,400 +2332,425 @@
   <dimension ref="A1:AZ66"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="14.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="5" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="5"/>
     <col min="7" max="7" width="9.140625" style="5" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="6">
+      <c r="B1" s="12"/>
+      <c r="C1" s="3">
         <v>4</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="J1" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="6">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="3">
         <v>36</v>
       </c>
-      <c r="O1" s="10"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="3"/>
       <c r="P1" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="Q1" s="10">
+      <c r="Q1" s="3">
         <f>'Motor Parameter Estimation'!B2</f>
         <v>0.115</v>
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="J2" s="17" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="J2" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="6">
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="3">
         <f>M1/C1</f>
         <v>9</v>
       </c>
-      <c r="O2" s="10"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="3"/>
       <c r="P2" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q2" s="3">
         <f>'Motor Parameter Estimation'!A2</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="6">
+      <c r="B3" s="12"/>
+      <c r="C3" s="3">
         <f>SIN(M3*N4/2)/(M3*SIN(N4/2))</f>
         <v>0.95979508052393891</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <f>SIN(3*M3*N4/2)/(M3*SIN(3*N4/2))</f>
         <v>0.66666666666666674</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <f>SIN(5*M3*N4/2)/(M3*SIN(5*N4/2))</f>
         <v>0.21756788155537973</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <f>SIN(7*M3*N4/2)/(M3*SIN(7*N4/2))</f>
         <v>-0.17736296207931862</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <f>SIN(9*M3*N4/2)/(M3*SIN(9*N4/2))</f>
         <v>-0.33333333333333331</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="6">
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="3">
         <f>M2/3</f>
         <v>3</v>
       </c>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="6">
+      <c r="B4" s="12"/>
+      <c r="C4" s="3">
         <f>M3*M5*C1/2</f>
         <v>180</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="J4" s="17" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="J4" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="6">
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="3">
         <f>180/M2</f>
         <v>20</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="3">
         <f>PI()/(180/M4)</f>
         <v>0.3490658503988659</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <f>('Motor Parameter Estimation'!D2*C6/M5)</f>
         <v>2.1769999999999996</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="G5" s="4"/>
+      <c r="J5" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="6">
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="3">
         <v>30</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="6">
+      <c r="B6" s="12"/>
+      <c r="C6" s="3">
         <v>0.7</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="J6" s="17" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="J6" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="9">
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="3">
         <f>(M3*M5*C1/2)</f>
         <v>180</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="3">
         <f>(C8/SQRT(3))/(4.44*C11*C3*N7)</f>
         <v>71.249819887081856</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="J7" s="17" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="J7" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="11">
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="4">
         <f>(C8/SQRT(3))/(4.44*C11*C3*M6)</f>
         <v>5.7203021630195597E-3</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="3">
         <f>N8*PI()*Q1*Q2/C1</f>
         <v>1.445132620651305E-2</v>
       </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="6">
+      <c r="B8" s="12"/>
+      <c r="C8" s="3">
         <v>380</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="J8" s="17" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="J8" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="9">
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="3">
         <f>M7/(PI()*Q1*Q2/C1)</f>
         <v>0.3166658661648083</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="3">
         <v>0.8</v>
       </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="6">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="J9" s="17" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="J9" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="10">
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="3">
         <v>1E-3</v>
       </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="6">
+      <c r="B10" s="12"/>
+      <c r="C10" s="3">
         <v>3000</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="J10" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="11">
-        <f>C10/M12</f>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="4">
+        <f>C10/M11</f>
         <v>20.462778397529405</v>
       </c>
-      <c r="N10" s="10">
-        <f>(0.5*M8^2*PI()*Q1^2*Q2/2)/(4*PI()*10^-7)</f>
-        <v>165.7708632811796</v>
-      </c>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="10">
+      <c r="B11" s="12"/>
+      <c r="C11" s="3">
         <v>50</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="J11" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="10">
-        <f>C10/N10</f>
-        <v>18.09726957210458</v>
-      </c>
-      <c r="N11" s="5">
-        <f>M11*60/(2*PI())</f>
-        <v>172.81619453201964</v>
-      </c>
-      <c r="O11" s="12" t="s">
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="3">
+        <f>2*PI()*N11/60</f>
+        <v>146.60765716752366</v>
+      </c>
+      <c r="N11" s="3">
+        <v>1400</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>125</v>
       </c>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="5">
+      <c r="B12" s="12"/>
+      <c r="C12" s="3">
         <f>C10/'Motor Parameter Estimation'!I2</f>
-        <v>3871.7081964643635</v>
-      </c>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="9">
-        <f>2*PI()*N12/60</f>
-        <v>146.60765716752366</v>
-      </c>
-      <c r="N12" s="9">
-        <v>1400</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>125</v>
-      </c>
+        <v>3308.1530331532981</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="14" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="13" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13" t="s">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13" t="s">
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13" t="s">
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13" t="s">
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13" t="s">
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13" t="s">
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13" t="s">
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13"/>
-      <c r="AB14" s="13" t="s">
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AC14" s="13"/>
-      <c r="AD14" s="13"/>
-      <c r="AE14" s="13" t="s">
+      <c r="AC14" s="12"/>
+      <c r="AD14" s="12"/>
+      <c r="AE14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AF14" s="13"/>
-      <c r="AG14" s="13"/>
-      <c r="AH14" s="13" t="s">
+      <c r="AF14" s="12"/>
+      <c r="AG14" s="12"/>
+      <c r="AH14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AI14" s="13"/>
-      <c r="AJ14" s="13"/>
+      <c r="AI14" s="12"/>
+      <c r="AJ14" s="12"/>
       <c r="AK14" s="1"/>
       <c r="AL14" s="1"/>
       <c r="AM14" s="1"/>
@@ -3258,72 +3280,72 @@
       </c>
     </row>
     <row r="61" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B61" s="8"/>
+      <c r="B61" s="7"/>
     </row>
     <row r="64" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="15"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="13" t="s">
+      <c r="B64" s="14"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13" t="s">
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13" t="s">
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K64" s="13"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="13" t="s">
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+      <c r="M64" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="N64" s="13"/>
-      <c r="O64" s="13"/>
-      <c r="P64" s="13" t="s">
+      <c r="N64" s="12"/>
+      <c r="O64" s="12"/>
+      <c r="P64" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="Q64" s="13"/>
-      <c r="R64" s="13"/>
-      <c r="S64" s="13" t="s">
+      <c r="Q64" s="12"/>
+      <c r="R64" s="12"/>
+      <c r="S64" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="T64" s="13"/>
-      <c r="U64" s="13"/>
-      <c r="V64" s="13" t="s">
+      <c r="T64" s="12"/>
+      <c r="U64" s="12"/>
+      <c r="V64" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="W64" s="13"/>
-      <c r="X64" s="13"/>
-      <c r="Y64" s="13" t="s">
+      <c r="W64" s="12"/>
+      <c r="X64" s="12"/>
+      <c r="Y64" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="Z64" s="13"/>
-      <c r="AA64" s="13"/>
-      <c r="AB64" s="13" t="s">
+      <c r="Z64" s="12"/>
+      <c r="AA64" s="12"/>
+      <c r="AB64" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AC64" s="13"/>
-      <c r="AD64" s="13"/>
-      <c r="AE64" s="13" t="s">
+      <c r="AC64" s="12"/>
+      <c r="AD64" s="12"/>
+      <c r="AE64" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AF64" s="13"/>
-      <c r="AG64" s="13"/>
-      <c r="AH64" s="13" t="s">
+      <c r="AF64" s="12"/>
+      <c r="AG64" s="12"/>
+      <c r="AH64" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AI64" s="13"/>
-      <c r="AJ64" s="13"/>
+      <c r="AI64" s="12"/>
+      <c r="AJ64" s="12"/>
       <c r="AK64" s="1"/>
       <c r="AL64" s="1"/>
       <c r="AM64" s="1"/>
@@ -3595,15 +3617,33 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="AH64:AJ64"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="J64:L64"/>
+    <mergeCell ref="M64:O64"/>
+    <mergeCell ref="P64:R64"/>
+    <mergeCell ref="S64:U64"/>
+    <mergeCell ref="V64:X64"/>
+    <mergeCell ref="Y64:AA64"/>
+    <mergeCell ref="AB64:AD64"/>
+    <mergeCell ref="AE64:AG64"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="AH14:AJ14"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="D14:F14"/>
@@ -3616,33 +3656,15 @@
     <mergeCell ref="Y14:AA14"/>
     <mergeCell ref="AB14:AD14"/>
     <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="AH64:AJ64"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="J64:L64"/>
-    <mergeCell ref="M64:O64"/>
-    <mergeCell ref="P64:R64"/>
-    <mergeCell ref="S64:U64"/>
-    <mergeCell ref="V64:X64"/>
-    <mergeCell ref="Y64:AA64"/>
-    <mergeCell ref="AB64:AD64"/>
-    <mergeCell ref="AE64:AG64"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3654,180 +3676,211 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="7"/>
-    <col min="3" max="3" width="25" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="30.5703125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="33.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="19.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="6"/>
+    <col min="3" max="3" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.5703125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="10" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="3">
         <v>0.2</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="3">
         <v>0.115</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="3">
         <v>0.17</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="3">
         <v>93.3</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="3">
         <f>'Winding Design'!M8</f>
         <v>0.3166658661648083</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="3">
         <v>1.5</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="3">
         <v>1.5</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="3">
         <f>L2/(11*E2*'Winding Design'!C3*I2*J2*10^-3)</f>
-        <v>16962.627505543849</v>
-      </c>
-      <c r="I2" s="7">
+        <v>16962.627505543845</v>
+      </c>
+      <c r="I2" s="3">
         <f>('Winding Design'!C10-(H5+D5+50))/'Winding Design'!C10</f>
-        <v>0.77485178318438208</v>
-      </c>
-      <c r="J2" s="7">
+        <v>0.90685042981232045</v>
+      </c>
+      <c r="J2" s="3">
         <v>0.8</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="3">
         <f>(120*50/'Winding Design'!C1)/60</f>
         <v>25</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="3">
         <f>(('Winding Design'!C10*I2)/(K2*M2))/1000</f>
-        <v>35.153956136909585</v>
-      </c>
-      <c r="M2" s="7">
+        <v>41.1425525812773</v>
+      </c>
+      <c r="M2" s="3">
         <f>B2^2*A2</f>
         <v>2.6450000000000002E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="10" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="3">
         <f>PI()*B2/'Winding Design'!C1</f>
         <v>9.0320788790706555E-2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="3">
         <f>2*A2+2.3*A5+0.24</f>
         <v>0.84773781421862504</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="3">
         <f>0.021*B5*'Winding Design'!M6/1.04</f>
         <v>3.0812009016792334</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="3">
         <f>3*'Winding Design'!C9^2*C5</f>
-        <v>591.59057312241282</v>
-      </c>
-      <c r="E5" s="10">
+        <v>195.59463323859771</v>
+      </c>
+      <c r="E5" s="3">
         <f>(('Winding Design'!M6^2)/('Winding Design'!M9/((2.5/1000)*A2*4*PI()*10^-7)))/10^-3</f>
         <v>20.357520395261858</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="3">
         <f>PI()*(C2/2)^2*A2*7850</f>
         <v>35.635870867832431</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="3">
         <f>G5*0.95</f>
         <v>33.854077324440809</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="3" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A5:D6">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{65605CF0-8A24-4652-8E8A-FE25475B23BD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{65605CF0-8A24-4652-8E8A-FE25475B23BD}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>A5:D6</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>